<commit_message>
Add ODK version form in exports
</commit_message>
<xml_diff>
--- a/inst/extdata/spa_hcpi_dict.xlsx
+++ b/inst/extdata/spa_hcpi_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="388">
   <si>
     <t>old</t>
   </si>
@@ -1182,6 +1182,12 @@
   </si>
   <si>
     <t>h5_8</t>
+  </si>
+  <si>
+    <t>FormVersion</t>
+  </si>
+  <si>
+    <t>form_version</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="79" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3445,6 +3451,17 @@
         <v>249</v>
       </c>
     </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>386</v>
+      </c>
+      <c r="B176" t="s">
+        <v>387</v>
+      </c>
+      <c r="C176" t="s">
+        <v>386</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>